<commit_message>
update gRPC for client
</commit_message>
<xml_diff>
--- a/resources/Inventory.xlsx
+++ b/resources/Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/Projects/Microservices/tedu-aspnetcore-microservices/tedu-aspnetcore-microservices/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{E3F0288E-6F67-BA4D-B4BA-CA00A8D0ADD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{C8DB4101-D92D-CC44-BFBA-91A33656D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69880" yWindow="-4520" windowWidth="32440" windowHeight="24540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="63900" yWindow="-4260" windowWidth="38240" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Purchase</t>
+  </si>
+  <si>
+    <t>SELECT ItemNo, Sum(Quantity) as Quantity FROM SaleOrders GROUP BY ItemNo</t>
+  </si>
+  <si>
+    <t>SELECT ItemNo, Sum(Quantity) as Quantity FROM PurchaseOrders GROUP BY ItemNo</t>
+  </si>
+  <si>
+    <t>SELECT ItemNo, Sum(Quantity) as Quantity FROM Inventory GROUP BY ItemNo</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
     <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="166" formatCode="[$£-809]#,##0.00;[Red][$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -235,6 +244,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF181818"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -379,7 +395,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -443,6 +459,12 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -500,6 +522,42 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -561,6 +619,108 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thick">
+          <color theme="3"/>
+        </top>
+        <bottom style="thick">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -626,6 +786,42 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -684,180 +880,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thick">
-          <color theme="3"/>
-        </top>
-        <bottom style="thick">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -949,10 +971,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PersonalItems" displayName="PersonalItems" ref="B12:E21" totalsRowCount="1">
   <autoFilter ref="B12:E20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="7" dataCellStyle="Item Description"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Document No" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Document Type" dataDxfId="17" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quantity" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="5" dataCellStyle="Item Description"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Document No" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Document Type" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quantity" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Personal inventory" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -967,10 +989,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{85EE672A-8B6B-D945-8654-7D90988FBE99}" name="PersonalItems4" displayName="PersonalItems4" ref="B12:E18" totalsRowCount="1">
   <autoFilter ref="B12:E17" xr:uid="{85EE672A-8B6B-D945-8654-7D90988FBE99}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2114A3E2-8E00-194F-B1B1-066BD8A11063}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="11" dataCellStyle="Item Description"/>
-    <tableColumn id="2" xr3:uid="{28F151B9-398D-B847-8246-211C9E35F244}" name="Document No" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A0CEF64B-6901-B24F-89E9-4DB654E0A15A}" name="Document Type" dataDxfId="15" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{C0818682-4EAC-1345-A2ED-0025B559FDEE}" name="Quantity" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{2114A3E2-8E00-194F-B1B1-066BD8A11063}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="17" dataCellStyle="Item Description"/>
+    <tableColumn id="2" xr3:uid="{28F151B9-398D-B847-8246-211C9E35F244}" name="Document No" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A0CEF64B-6901-B24F-89E9-4DB654E0A15A}" name="Document Type" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{C0818682-4EAC-1345-A2ED-0025B559FDEE}" name="Quantity" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Personal inventory" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -985,10 +1007,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{02FF2381-E98D-1A45-B959-2A39843E0F9F}" name="PersonalItems45" displayName="PersonalItems45" ref="B12:E16" totalsRowCount="1">
   <autoFilter ref="B12:E15" xr:uid="{02FF2381-E98D-1A45-B959-2A39843E0F9F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9D02A5C9-7B7C-3546-9722-A5FD3C77AD0E}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="3" dataCellStyle="Item Description"/>
-    <tableColumn id="2" xr3:uid="{B27F5994-E9FD-D541-9308-1E141723ADE8}" name="Document No" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{58B04A58-BA33-7040-A4FC-658D43C29FA5}" name="Document Type" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D160855E-99AF-514A-BE02-59D5246E8EC0}" name="Quantity" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{9D02A5C9-7B7C-3546-9722-A5FD3C77AD0E}" name="Item No" totalsRowLabel="Total" totalsRowDxfId="11" dataCellStyle="Item Description"/>
+    <tableColumn id="2" xr3:uid="{B27F5994-E9FD-D541-9308-1E141723ADE8}" name="Document No" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{58B04A58-BA33-7040-A4FC-658D43C29FA5}" name="Document Type" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{D160855E-99AF-514A-BE02-59D5246E8EC0}" name="Quantity" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Personal inventory" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1206,10 +1228,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G14" sqref="G13:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1375,7 +1397,7 @@
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>30</v>
@@ -1389,7 +1411,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>29</v>
@@ -1403,7 +1425,7 @@
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>29</v>
@@ -1417,7 +1439,7 @@
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>29</v>
@@ -1431,7 +1453,7 @@
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>30</v>
@@ -1445,7 +1467,7 @@
     </row>
     <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>29</v>
@@ -1459,13 +1481,13 @@
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="19">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="21">
         <v>-5</v>
@@ -1483,8 +1505,19 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="B23:E23"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{76C29AD8-D006-6E4D-8A17-8FBB7A44F055}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{D51F5C92-AB51-CA4A-88EC-4310E6098691}"/>
@@ -1503,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F19C5ECC-D669-D447-9D18-B54A41430734}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1705,7 @@
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
@@ -1686,7 +1719,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>29</v>
@@ -1700,7 +1733,7 @@
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>29</v>
@@ -1714,7 +1747,7 @@
     </row>
     <row r="17" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>29</v>
@@ -1738,7 +1771,18 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B20:E20"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{0B194B64-9BD8-984F-8A62-B9E7C0573DA3}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{A6E00D0C-6771-344C-A27A-0FCFA04E7505}"/>
@@ -1752,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B0F21B-407E-CA40-9C32-7A6B364E19D6}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1907,7 +1951,7 @@
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>30</v>
@@ -1921,7 +1965,7 @@
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>30</v>
@@ -1935,7 +1979,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>30</v>
@@ -1958,8 +2002,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:E18"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{22AE8CB0-98A9-2F43-B4B1-8F5EEF7E1F7A}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{3426F882-9E16-3049-A52C-7D20432284CB}"/>

</xml_diff>